<commit_message>
Added Conditional Formatting for negative numbers
</commit_message>
<xml_diff>
--- a/Weapon_Damage.xlsx
+++ b/Weapon_Damage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\ERRP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4970105-B6CE-47BE-B6B9-22125B4A5616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0846A198-4400-4320-B6C0-CF25623193C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{E04E184C-43B9-435F-A69D-D6A5B308AEAE}"/>
   </bookViews>
@@ -679,7 +679,52 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -3104,7 +3149,7 @@
   <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="F2" sqref="F2:F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5761,6 +5806,48 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{BE4F84B5-271F-47AA-B4C3-2B3874F7B411}">
+            <xm:f>NOT(ISERROR(SEARCH("-",B4)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+                <i val="0"/>
+                <color theme="0"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>B4:B21 B25:B42 B46:B53 B57:B66 B70:B81 B85:B88 B92:B96 B100:B109 B113:B122 B126:B127</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{46892EE9-9600-49B6-8D93-518CC33F69A2}">
+            <xm:f>NOT(ISERROR(SEARCH("-",F4)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F4:F21 F25:F42 F46:F53 F57:F66 F70:F81 F85:F88 F92:F96 F100:F109 F113:F122 F126:F128</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>